<commit_message>
chore(tool_output): :bug: fixing example anonymized files
</commit_message>
<xml_diff>
--- a/files/tool_output/03_anwers_and_califications_dataframe/answers.xlsx
+++ b/files/tool_output/03_anwers_and_califications_dataframe/answers.xlsx
@@ -537,22 +537,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ABRAHAM MURPHY</t>
+          <t>user87</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ABRAHAM MURPHY</t>
+          <t>user87</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ABRAHAM MURPHY</t>
+          <t>user87</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ABRAHAM MURPHY</t>
+          <t>user87</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -637,22 +637,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GARRY CAMERON</t>
+          <t>user39</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GARRY CAMERON</t>
+          <t>user39</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GARRY CAMERON</t>
+          <t>user39</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GARRY CAMERON</t>
+          <t>user39</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -733,22 +733,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DANIEL CAMPBELL</t>
+          <t>user3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DANIEL CAMPBELL</t>
+          <t>user3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DANIEL CAMPBELL</t>
+          <t>user3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>DANIEL CAMPBELL</t>
+          <t>user3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -828,22 +828,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MYRA MILLER</t>
+          <t>user95</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MYRA MILLER</t>
+          <t>user95</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MYRA MILLER</t>
+          <t>user95</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MYRA MILLER</t>
+          <t>user95</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -923,22 +923,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NATALIE HAMILTON</t>
+          <t>user101</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NATALIE HAMILTON</t>
+          <t>user101</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NATALIE HAMILTON</t>
+          <t>user101</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>NATALIE HAMILTON</t>
+          <t>user101</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1020,22 +1020,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AUDREY DIXON</t>
+          <t>user36</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AUDREY DIXON</t>
+          <t>user36</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AUDREY DIXON</t>
+          <t>user36</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>AUDREY DIXON</t>
+          <t>user36</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1113,22 +1113,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MAXIMILIAN HUNT</t>
+          <t>user58</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MAXIMILIAN HUNT</t>
+          <t>user58</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MAXIMILIAN HUNT</t>
+          <t>user58</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MAXIMILIAN HUNT</t>
+          <t>user58</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1209,22 +1209,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FREDDIE ELLIOTT</t>
+          <t>user97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FREDDIE ELLIOTT</t>
+          <t>user97</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FREDDIE ELLIOTT</t>
+          <t>user97</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FREDDIE ELLIOTT</t>
+          <t>user97</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1305,22 +1305,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GIANNA ROSS</t>
+          <t>user85</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>GIANNA ROSS</t>
+          <t>user85</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>GIANNA ROSS</t>
+          <t>user85</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>GIANNA ROSS</t>
+          <t>user85</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1404,22 +1404,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ABIGAIL CASEY</t>
+          <t>user69</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ABIGAIL CASEY</t>
+          <t>user69</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ABIGAIL CASEY</t>
+          <t>user69</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ABIGAIL CASEY</t>
+          <t>user69</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1502,22 +1502,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>FIONA HOWARD</t>
+          <t>user74</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>FIONA HOWARD</t>
+          <t>user74</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>FIONA HOWARD</t>
+          <t>user74</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FIONA HOWARD</t>
+          <t>user74</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1599,22 +1599,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LUCIA TUCKER</t>
+          <t>user44</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LUCIA TUCKER</t>
+          <t>user44</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>LUCIA TUCKER</t>
+          <t>user44</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>LUCIA TUCKER</t>
+          <t>user44</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1700,22 +1700,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LUCAS BARRETT</t>
+          <t>user63</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LUCAS BARRETT</t>
+          <t>user63</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LUCAS BARRETT</t>
+          <t>user63</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>LUCAS BARRETT</t>
+          <t>user63</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1801,22 +1801,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>LUCAS HALL</t>
+          <t>user37</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LUCAS HALL</t>
+          <t>user37</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LUCAS HALL</t>
+          <t>user37</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>LUCAS HALL</t>
+          <t>user37</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1899,22 +1899,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AIDA MOORE</t>
+          <t>user102</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AIDA MOORE</t>
+          <t>user102</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>AIDA MOORE</t>
+          <t>user102</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>AIDA MOORE</t>
+          <t>user102</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1997,22 +1997,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ALFRED HAMILTON</t>
+          <t>user62</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ALFRED HAMILTON</t>
+          <t>user62</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ALFRED HAMILTON</t>
+          <t>user62</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ALFRED HAMILTON</t>
+          <t>user62</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -2094,22 +2094,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SPIKE MITCHELL</t>
+          <t>user56</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SPIKE MITCHELL</t>
+          <t>user56</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>SPIKE MITCHELL</t>
+          <t>user56</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>SPIKE MITCHELL</t>
+          <t>user56</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2198,22 +2198,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SOPHIA HOWARD</t>
+          <t>user47</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SOPHIA HOWARD</t>
+          <t>user47</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SOPHIA HOWARD</t>
+          <t>user47</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>SOPHIA HOWARD</t>
+          <t>user47</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2299,22 +2299,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NATALIE RICHARDS</t>
+          <t>user80</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>NATALIE RICHARDS</t>
+          <t>user80</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>NATALIE RICHARDS</t>
+          <t>user80</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>NATALIE RICHARDS</t>
+          <t>user80</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2396,22 +2396,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CARINA HAWKINS</t>
+          <t>user65</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CARINA HAWKINS</t>
+          <t>user65</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CARINA HAWKINS</t>
+          <t>user65</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>CARINA HAWKINS</t>
+          <t>user65</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2493,22 +2493,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ADELAIDE KELLY</t>
+          <t>user13</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ADELAIDE KELLY</t>
+          <t>user13</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ADELAIDE KELLY</t>
+          <t>user13</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ADELAIDE KELLY</t>
+          <t>user13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2591,22 +2591,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>OLIVER FARRELL</t>
+          <t>user71</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OLIVER FARRELL</t>
+          <t>user71</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OLIVER FARRELL</t>
+          <t>user71</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>OLIVER FARRELL</t>
+          <t>user71</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2692,22 +2692,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ELIAN PERRY</t>
+          <t>user99</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ELIAN PERRY</t>
+          <t>user99</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ELIAN PERRY</t>
+          <t>user99</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ELIAN PERRY</t>
+          <t>user99</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2790,22 +2790,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>JASMINE DOUGLAS</t>
+          <t>user48</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>JASMINE DOUGLAS</t>
+          <t>user48</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>JASMINE DOUGLAS</t>
+          <t>user48</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>JASMINE DOUGLAS</t>
+          <t>user48</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2886,22 +2886,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CARL DAVIS</t>
+          <t>user92</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CARL DAVIS</t>
+          <t>user92</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CARL DAVIS</t>
+          <t>user92</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CARL DAVIS</t>
+          <t>user92</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2984,22 +2984,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BELINDA MURPHY</t>
+          <t>user7</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BELINDA MURPHY</t>
+          <t>user7</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>BELINDA MURPHY</t>
+          <t>user7</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>BELINDA MURPHY</t>
+          <t>user7</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -3080,22 +3080,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BELINDA PARKER</t>
+          <t>user51</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BELINDA PARKER</t>
+          <t>user51</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>BELINDA PARKER</t>
+          <t>user51</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>BELINDA PARKER</t>
+          <t>user51</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3180,22 +3180,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>NATALIE COLE</t>
+          <t>user28</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NATALIE COLE</t>
+          <t>user28</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>NATALIE COLE</t>
+          <t>user28</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>NATALIE COLE</t>
+          <t>user28</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -3272,22 +3272,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GARRY KELLY</t>
+          <t>user60</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>GARRY KELLY</t>
+          <t>user60</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>GARRY KELLY</t>
+          <t>user60</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>GARRY KELLY</t>
+          <t>user60</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -3369,22 +3369,22 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ALDUS THOMPSON</t>
+          <t>user45</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ALDUS THOMPSON</t>
+          <t>user45</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ALDUS THOMPSON</t>
+          <t>user45</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ALDUS THOMPSON</t>
+          <t>user45</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -3463,22 +3463,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>EVELYN ELLIOTT</t>
+          <t>user96</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>EVELYN ELLIOTT</t>
+          <t>user96</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>EVELYN ELLIOTT</t>
+          <t>user96</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>EVELYN ELLIOTT</t>
+          <t>user96</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -3561,22 +3561,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LYDIA JOHNSON</t>
+          <t>user77</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LYDIA JOHNSON</t>
+          <t>user77</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>LYDIA JOHNSON</t>
+          <t>user77</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>LYDIA JOHNSON</t>
+          <t>user77</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -3656,22 +3656,22 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MAX WELLS</t>
+          <t>user64</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MAX WELLS</t>
+          <t>user64</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MAX WELLS</t>
+          <t>user64</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>MAX WELLS</t>
+          <t>user64</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -3750,22 +3750,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CHERRY HUNT</t>
+          <t>user17</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CHERRY HUNT</t>
+          <t>user17</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CHERRY HUNT</t>
+          <t>user17</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>CHERRY HUNT</t>
+          <t>user17</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -3843,22 +3843,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>MARCUS MILLER</t>
+          <t>user50</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MARCUS MILLER</t>
+          <t>user50</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MARCUS MILLER</t>
+          <t>user50</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>MARCUS MILLER</t>
+          <t>user50</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -3942,22 +3942,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>HENRY ROSS</t>
+          <t>user1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HENRY ROSS</t>
+          <t>user1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>HENRY ROSS</t>
+          <t>user1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>HENRY ROSS</t>
+          <t>user1</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -4041,22 +4041,22 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ASHTON MOORE</t>
+          <t>user4</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ASHTON MOORE</t>
+          <t>user4</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ASHTON MOORE</t>
+          <t>user4</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ASHTON MOORE</t>
+          <t>user4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -4139,22 +4139,22 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ALBERTA WATSON</t>
+          <t>user89</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ALBERTA WATSON</t>
+          <t>user89</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ALBERTA WATSON</t>
+          <t>user89</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ALBERTA WATSON</t>
+          <t>user89</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -4231,22 +4231,22 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>user84</t>
+          <t>UTRERA LOPEZ</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>user84</t>
+          <t>MARINA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>user84</t>
+          <t>0139513</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>user84</t>
+          <t>marina.utreralopez@alum.uca.es</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -4330,22 +4330,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>REBECCA PERKINS</t>
+          <t>user40</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>REBECCA PERKINS</t>
+          <t>user40</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>REBECCA PERKINS</t>
+          <t>user40</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>REBECCA PERKINS</t>
+          <t>user40</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -4427,22 +4427,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>JENNA WARREN</t>
+          <t>user75</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>JENNA WARREN</t>
+          <t>user75</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>JENNA WARREN</t>
+          <t>user75</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>JENNA WARREN</t>
+          <t>user75</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -4524,22 +4524,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>KELLAN CUNNINGHAM</t>
+          <t>user5</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>KELLAN CUNNINGHAM</t>
+          <t>user5</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>KELLAN CUNNINGHAM</t>
+          <t>user5</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>KELLAN CUNNINGHAM</t>
+          <t>user5</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -4624,22 +4624,22 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ARNOLD JOHNSON</t>
+          <t>user84</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ARNOLD JOHNSON</t>
+          <t>user84</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ARNOLD JOHNSON</t>
+          <t>user84</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ARNOLD JOHNSON</t>
+          <t>user84</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -4723,22 +4723,22 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ADRIAN RILEY</t>
+          <t>user20</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ADRIAN RILEY</t>
+          <t>user20</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ADRIAN RILEY</t>
+          <t>user20</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>ADRIAN RILEY</t>
+          <t>user20</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -4822,22 +4822,22 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>OSCAR ANDREWS</t>
+          <t>user98</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>OSCAR ANDREWS</t>
+          <t>user98</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>OSCAR ANDREWS</t>
+          <t>user98</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>OSCAR ANDREWS</t>
+          <t>user98</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -4918,22 +4918,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>JAMES TAYLOR</t>
+          <t>user24</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>JAMES TAYLOR</t>
+          <t>user24</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>JAMES TAYLOR</t>
+          <t>user24</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>JAMES TAYLOR</t>
+          <t>user24</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -5013,22 +5013,22 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>SABRINA HARRIS</t>
+          <t>user38</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SABRINA HARRIS</t>
+          <t>user38</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SABRINA HARRIS</t>
+          <t>user38</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>SABRINA HARRIS</t>
+          <t>user38</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -5109,22 +5109,22 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ALBERT CUNNINGHAM</t>
+          <t>user29</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALBERT CUNNINGHAM</t>
+          <t>user29</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ALBERT CUNNINGHAM</t>
+          <t>user29</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ALBERT CUNNINGHAM</t>
+          <t>user29</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -5203,22 +5203,22 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>GRACE TUCKER</t>
+          <t>user25</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>GRACE TUCKER</t>
+          <t>user25</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>GRACE TUCKER</t>
+          <t>user25</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>GRACE TUCKER</t>
+          <t>user25</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -5302,22 +5302,22 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>STUART HENDERSON</t>
+          <t>user42</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>STUART HENDERSON</t>
+          <t>user42</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>STUART HENDERSON</t>
+          <t>user42</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>STUART HENDERSON</t>
+          <t>user42</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -5402,22 +5402,22 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CHARLIE PERRY</t>
+          <t>user12</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>CHARLIE PERRY</t>
+          <t>user12</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CHARLIE PERRY</t>
+          <t>user12</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>CHARLIE PERRY</t>
+          <t>user12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -5500,22 +5500,22 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>LYNDON HALL</t>
+          <t>user54</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>LYNDON HALL</t>
+          <t>user54</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>LYNDON HALL</t>
+          <t>user54</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>LYNDON HALL</t>
+          <t>user54</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -5602,22 +5602,22 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>MADDIE ROBINSON</t>
+          <t>user9</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>MADDIE ROBINSON</t>
+          <t>user9</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MADDIE ROBINSON</t>
+          <t>user9</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>MADDIE ROBINSON</t>
+          <t>user9</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -5705,22 +5705,22 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>VIVIAN PAYNE</t>
+          <t>user27</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>VIVIAN PAYNE</t>
+          <t>user27</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>VIVIAN PAYNE</t>
+          <t>user27</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>VIVIAN PAYNE</t>
+          <t>user27</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -5812,22 +5812,22 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>LEONARDO BAILEY</t>
+          <t>user82</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>LEONARDO BAILEY</t>
+          <t>user82</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>LEONARDO BAILEY</t>
+          <t>user82</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>LEONARDO BAILEY</t>
+          <t>user82</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -5906,22 +5906,22 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CONNIE PHILLIPS</t>
+          <t>user81</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>CONNIE PHILLIPS</t>
+          <t>user81</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CONNIE PHILLIPS</t>
+          <t>user81</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>CONNIE PHILLIPS</t>
+          <t>user81</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -6003,22 +6003,22 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>JULIAN EVANS</t>
+          <t>user15</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>JULIAN EVANS</t>
+          <t>user15</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>JULIAN EVANS</t>
+          <t>user15</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>JULIAN EVANS</t>
+          <t>user15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -6102,22 +6102,22 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>SAM CAMERON</t>
+          <t>user10</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>SAM CAMERON</t>
+          <t>user10</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SAM CAMERON</t>
+          <t>user10</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>SAM CAMERON</t>
+          <t>user10</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -6203,22 +6203,22 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ALFORD FERGUSON</t>
+          <t>user32</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ALFORD FERGUSON</t>
+          <t>user32</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ALFORD FERGUSON</t>
+          <t>user32</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>ALFORD FERGUSON</t>
+          <t>user32</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -6300,22 +6300,22 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>CARLOS MARTIN</t>
+          <t>user104</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>CARLOS MARTIN</t>
+          <t>user104</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>CARLOS MARTIN</t>
+          <t>user104</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>CARLOS MARTIN</t>
+          <t>user104</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -6402,22 +6402,22 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MARCUS MORGAN</t>
+          <t>user76</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>MARCUS MORGAN</t>
+          <t>user76</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>MARCUS MORGAN</t>
+          <t>user76</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>MARCUS MORGAN</t>
+          <t>user76</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -6495,22 +6495,22 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>RYAN HARRIS</t>
+          <t>user59</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>RYAN HARRIS</t>
+          <t>user59</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>RYAN HARRIS</t>
+          <t>user59</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>RYAN HARRIS</t>
+          <t>user59</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -6598,22 +6598,22 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ALEN CAMPBELL</t>
+          <t>user93</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>ALEN CAMPBELL</t>
+          <t>user93</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ALEN CAMPBELL</t>
+          <t>user93</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>ALEN CAMPBELL</t>
+          <t>user93</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -6691,22 +6691,22 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>VICTOR JOHNSON</t>
+          <t>user11</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>VICTOR JOHNSON</t>
+          <t>user11</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>VICTOR JOHNSON</t>
+          <t>user11</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>VICTOR JOHNSON</t>
+          <t>user11</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -6788,22 +6788,22 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>CARLOS HAWKINS</t>
+          <t>user91</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>CARLOS HAWKINS</t>
+          <t>user91</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CARLOS HAWKINS</t>
+          <t>user91</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>CARLOS HAWKINS</t>
+          <t>user91</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -6885,22 +6885,22 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>OWEN FOSTER</t>
+          <t>user35</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>OWEN FOSTER</t>
+          <t>user35</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>OWEN FOSTER</t>
+          <t>user35</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>OWEN FOSTER</t>
+          <t>user35</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -6984,22 +6984,22 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BROOKE HOWARD</t>
+          <t>user22</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>BROOKE HOWARD</t>
+          <t>user22</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BROOKE HOWARD</t>
+          <t>user22</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>BROOKE HOWARD</t>
+          <t>user22</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -7087,22 +7087,22 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>DEXTER HILL</t>
+          <t>user21</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>DEXTER HILL</t>
+          <t>user21</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>DEXTER HILL</t>
+          <t>user21</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>DEXTER HILL</t>
+          <t>user21</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -7189,22 +7189,22 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>FREDERICK PARKER</t>
+          <t>user70</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>FREDERICK PARKER</t>
+          <t>user70</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>FREDERICK PARKER</t>
+          <t>user70</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>FREDERICK PARKER</t>
+          <t>user70</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -7284,22 +7284,22 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>LILY MURPHY</t>
+          <t>user61</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>LILY MURPHY</t>
+          <t>user61</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>LILY MURPHY</t>
+          <t>user61</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>LILY MURPHY</t>
+          <t>user61</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -7387,22 +7387,22 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ALAN WRIGHT</t>
+          <t>user94</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>ALAN WRIGHT</t>
+          <t>user94</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ALAN WRIGHT</t>
+          <t>user94</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>ALAN WRIGHT</t>
+          <t>user94</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -7484,22 +7484,22 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ANNA HARPER</t>
+          <t>user18</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>ANNA HARPER</t>
+          <t>user18</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>ANNA HARPER</t>
+          <t>user18</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>ANNA HARPER</t>
+          <t>user18</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -7586,22 +7586,22 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>SOPHIA HALL</t>
+          <t>user88</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SOPHIA HALL</t>
+          <t>user88</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SOPHIA HALL</t>
+          <t>user88</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>SOPHIA HALL</t>
+          <t>user88</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -7682,22 +7682,22 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>LUKE THOMAS</t>
+          <t>user73</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>LUKE THOMAS</t>
+          <t>user73</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LUKE THOMAS</t>
+          <t>user73</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>LUKE THOMAS</t>
+          <t>user73</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -7779,22 +7779,22 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>GEORGE EDWARDS</t>
+          <t>user16</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>GEORGE EDWARDS</t>
+          <t>user16</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>GEORGE EDWARDS</t>
+          <t>user16</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>GEORGE EDWARDS</t>
+          <t>user16</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -7876,22 +7876,22 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>LUCIA ELLIS</t>
+          <t>user6</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>LUCIA ELLIS</t>
+          <t>user6</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>LUCIA ELLIS</t>
+          <t>user6</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>LUCIA ELLIS</t>
+          <t>user6</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -7973,22 +7973,22 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>FREDDIE WILLIAMS</t>
+          <t>user2</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>FREDDIE WILLIAMS</t>
+          <t>user2</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>FREDDIE WILLIAMS</t>
+          <t>user2</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>FREDDIE WILLIAMS</t>
+          <t>user2</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -8071,22 +8071,22 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>CATHERINE JONES</t>
+          <t>user23</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>CATHERINE JONES</t>
+          <t>user23</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>CATHERINE JONES</t>
+          <t>user23</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>CATHERINE JONES</t>
+          <t>user23</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -8175,22 +8175,22 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>JACK ALEXANDER</t>
+          <t>user41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>JACK ALEXANDER</t>
+          <t>user41</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>JACK ALEXANDER</t>
+          <t>user41</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>JACK ALEXANDER</t>
+          <t>user41</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -8271,22 +8271,22 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>TED CRAIG</t>
+          <t>user57</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>TED CRAIG</t>
+          <t>user57</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>TED CRAIG</t>
+          <t>user57</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>TED CRAIG</t>
+          <t>user57</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -8371,22 +8371,22 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>EDGAR JOHNSTON</t>
+          <t>user26</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>EDGAR JOHNSTON</t>
+          <t>user26</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>EDGAR JOHNSTON</t>
+          <t>user26</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>EDGAR JOHNSTON</t>
+          <t>user26</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -8466,22 +8466,22 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>MAYA ALLEN</t>
+          <t>user105</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>MAYA ALLEN</t>
+          <t>user105</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>MAYA ALLEN</t>
+          <t>user105</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>MAYA ALLEN</t>
+          <t>user105</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -8568,22 +8568,22 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>FENTON MARTIN</t>
+          <t>user86</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>FENTON MARTIN</t>
+          <t>user86</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>FENTON MARTIN</t>
+          <t>user86</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>FENTON MARTIN</t>
+          <t>user86</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -8666,22 +8666,22 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>TYLER MASON</t>
+          <t>user8</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>TYLER MASON</t>
+          <t>user8</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>TYLER MASON</t>
+          <t>user8</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>TYLER MASON</t>
+          <t>user8</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -8763,22 +8763,22 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ROLAND MONTGOMERY</t>
+          <t>user83</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ROLAND MONTGOMERY</t>
+          <t>user83</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>ROLAND MONTGOMERY</t>
+          <t>user83</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>ROLAND MONTGOMERY</t>
+          <t>user83</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -8865,22 +8865,22 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>EVELYN MARTIN</t>
+          <t>user43</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>EVELYN MARTIN</t>
+          <t>user43</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>EVELYN MARTIN</t>
+          <t>user43</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>EVELYN MARTIN</t>
+          <t>user43</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -8961,22 +8961,22 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>SOFIA CUNNINGHAM</t>
+          <t>user78</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>SOFIA CUNNINGHAM</t>
+          <t>user78</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>SOFIA CUNNINGHAM</t>
+          <t>user78</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>SOFIA CUNNINGHAM</t>
+          <t>user78</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -9056,22 +9056,22 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>VIOLET REED</t>
+          <t>user46</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>VIOLET REED</t>
+          <t>user46</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>VIOLET REED</t>
+          <t>user46</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>VIOLET REED</t>
+          <t>user46</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -9157,22 +9157,22 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>CARLOS TAYLOR</t>
+          <t>user67</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>CARLOS TAYLOR</t>
+          <t>user67</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>CARLOS TAYLOR</t>
+          <t>user67</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>CARLOS TAYLOR</t>
+          <t>user67</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -9254,22 +9254,22 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>KELLAN BAKER</t>
+          <t>user66</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>KELLAN BAKER</t>
+          <t>user66</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>KELLAN BAKER</t>
+          <t>user66</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>KELLAN BAKER</t>
+          <t>user66</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -9347,22 +9347,22 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ROBERT WILSON</t>
+          <t>user55</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>ROBERT WILSON</t>
+          <t>user55</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>ROBERT WILSON</t>
+          <t>user55</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>ROBERT WILSON</t>
+          <t>user55</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -9443,22 +9443,22 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>FENTON MITCHELL</t>
+          <t>user103</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>FENTON MITCHELL</t>
+          <t>user103</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>FENTON MITCHELL</t>
+          <t>user103</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>FENTON MITCHELL</t>
+          <t>user103</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -9542,22 +9542,22 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>FIONA KELLY</t>
+          <t>user68</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>FIONA KELLY</t>
+          <t>user68</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>FIONA KELLY</t>
+          <t>user68</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>FIONA KELLY</t>
+          <t>user68</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -9635,22 +9635,22 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>KATE BARNES</t>
+          <t>user52</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>KATE BARNES</t>
+          <t>user52</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>KATE BARNES</t>
+          <t>user52</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>KATE BARNES</t>
+          <t>user52</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -9732,22 +9732,22 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>LENNY MONTGOMERY</t>
+          <t>user33</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>LENNY MONTGOMERY</t>
+          <t>user33</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>LENNY MONTGOMERY</t>
+          <t>user33</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>LENNY MONTGOMERY</t>
+          <t>user33</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -9838,22 +9838,22 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>RYAN ROBERTS</t>
+          <t>user100</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>RYAN ROBERTS</t>
+          <t>user100</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>RYAN ROBERTS</t>
+          <t>user100</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>RYAN ROBERTS</t>
+          <t>user100</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -9945,22 +9945,22 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>EDDY BENNETT</t>
+          <t>user34</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>EDDY BENNETT</t>
+          <t>user34</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>EDDY BENNETT</t>
+          <t>user34</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>EDDY BENNETT</t>
+          <t>user34</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -10047,22 +10047,22 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>LILY ANDERSON</t>
+          <t>user53</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>LILY ANDERSON</t>
+          <t>user53</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>LILY ANDERSON</t>
+          <t>user53</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>LILY ANDERSON</t>
+          <t>user53</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -10142,22 +10142,22 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>PENELOPE ROBERTS</t>
+          <t>user19</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>PENELOPE ROBERTS</t>
+          <t>user19</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>PENELOPE ROBERTS</t>
+          <t>user19</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>PENELOPE ROBERTS</t>
+          <t>user19</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -10238,22 +10238,22 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>HEATHER SCOTT</t>
+          <t>user72</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>HEATHER SCOTT</t>
+          <t>user72</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>HEATHER SCOTT</t>
+          <t>user72</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>HEATHER SCOTT</t>
+          <t>user72</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -10337,22 +10337,22 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>TED BROOKS</t>
+          <t>user79</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>TED BROOKS</t>
+          <t>user79</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>TED BROOKS</t>
+          <t>user79</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>TED BROOKS</t>
+          <t>user79</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -10437,22 +10437,22 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>EVELYN MURPHY</t>
+          <t>user90</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>EVELYN MURPHY</t>
+          <t>user90</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>EVELYN MURPHY</t>
+          <t>user90</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>EVELYN MURPHY</t>
+          <t>user90</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">

</xml_diff>